<commit_message>
additional changes, especially to front-area pieces, as well as addition of finalized pieces, relative to acrylic order from 04.15.2013
</commit_message>
<xml_diff>
--- a/instructions/behav_rig_specs_final.xlsx
+++ b/instructions/behav_rig_specs_final.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37280" yWindow="-60" windowWidth="31960" windowHeight="19660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-27740" yWindow="5500" windowWidth="23500" windowHeight="12860" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="acrylic pieces" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="362">
   <si>
     <t>Base</t>
   </si>
@@ -465,9 +465,6 @@
   </si>
   <si>
     <t>Front Panel Frame (tapped, M3, x4)</t>
-  </si>
-  <si>
-    <t>side door (attachment) (M6 thumb screw)</t>
   </si>
   <si>
     <t>lick spout holder (tapped, M2.5, x2)</t>
@@ -1036,18 +1033,9 @@
     <t>**side_door_slotted (4 M3 tapped)</t>
   </si>
   <si>
-    <t>**new piece.</t>
-  </si>
-  <si>
-    <t>(same as other door piece)</t>
-  </si>
-  <si>
     <t>b1*, 1x</t>
   </si>
   <si>
-    <t>b1* (12x16), 1x -- GET IN CLEAR-RED ACRYLIC, 1/8" if possible</t>
-  </si>
-  <si>
     <t>12" x 16"</t>
   </si>
   <si>
@@ -1066,21 +1054,12 @@
     <t>*changed</t>
   </si>
   <si>
-    <t>*new</t>
-  </si>
-  <si>
     <t>black 1/4" acrylic (17.5"x9")</t>
   </si>
   <si>
     <t>black 1/4" acrylic (12.5"x16.5")</t>
   </si>
   <si>
-    <t>black 1/8" acrylic (12"x16")</t>
-  </si>
-  <si>
-    <t>clear-red 1/8" acrylic (12"x16")</t>
-  </si>
-  <si>
     <t>B4</t>
   </si>
   <si>
@@ -1091,13 +1070,73 @@
   </si>
   <si>
     <t>PIECE</t>
+  </si>
+  <si>
+    <t>[for 8 doors, 8 monitor mounts]</t>
+  </si>
+  <si>
+    <t>[for 16 side_door_frames]</t>
+  </si>
+  <si>
+    <t>[1 more, plus 8 extra, in case replaced]</t>
+  </si>
+  <si>
+    <t>*new [get 8, OR get 16, if replace all]</t>
+  </si>
+  <si>
+    <t>r1* (12x16), 1x -- GET IN CLEAR-RED ACRYLIC, 1/8" if possible</t>
+  </si>
+  <si>
+    <t>*15 (short version)</t>
+  </si>
+  <si>
+    <t>clear-red 1/8" acrylic (12"x15")</t>
+  </si>
+  <si>
+    <t>black 1/8" acrylic (12"x15")</t>
+  </si>
+  <si>
+    <t>Need:</t>
+  </si>
+  <si>
+    <t>*needed amount + 4 extra of each piece (except black 1/8")</t>
+  </si>
+  <si>
+    <t>36 x 8 ft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48" </t>
+  </si>
+  <si>
+    <t>48 x 96</t>
+  </si>
+  <si>
+    <t>4 setups</t>
+  </si>
+  <si>
+    <t>3 setups</t>
+  </si>
+  <si>
+    <t>24 pieces</t>
+  </si>
+  <si>
+    <t>20 (sheet makes 24)</t>
+  </si>
+  <si>
+    <t>[sideDoorAttachment_v4 is the shorter panel -- use this]</t>
+  </si>
+  <si>
+    <t>(curr: side_door_slotted_v1 -- make slot smaller)</t>
+  </si>
+  <si>
+    <t>side door (attachment) (M6 thumb or 4 M3 tapped)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1137,14 +1176,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="1"/>
@@ -1166,6 +1197,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1181,11 +1226,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1310,23 +1355,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1351,99 +1381,103 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1468,19 +1502,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="23"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="24"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="114"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="114" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="119">
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="24" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1492,51 +1526,54 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="114" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1548,51 +1585,53 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2755,7 +2794,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2766,7 +2805,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2782,105 +2821,105 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
         <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
         <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B10" t="s">
         <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B13" t="s">
         <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B14" t="s">
         <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B15" t="s">
         <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B16" t="s">
         <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B17" t="s">
         <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B18" t="s">
         <v>83</v>
@@ -2891,18 +2930,18 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B21" t="s">
         <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2913,28 +2952,28 @@
         <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="D23" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B24" t="s">
         <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B25" t="s">
         <v>83</v>
@@ -2942,18 +2981,18 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B26" t="s">
         <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B28" t="s">
         <v>83</v>
@@ -2961,7 +3000,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B29" t="s">
         <v>85</v>
@@ -2969,45 +3008,45 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B31" t="s">
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B32" t="s">
         <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B35" t="s">
         <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -3015,18 +3054,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B41" t="s">
         <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -3045,33 +3084,33 @@
         <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B46" t="s">
         <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3089,7 +3128,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B53" t="s">
         <v>86</v>
@@ -3097,7 +3136,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3105,7 +3144,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -3119,20 +3158,20 @@
         <v>86</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="25"/>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="C60" s="25" t="s">
         <v>284</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>285</v>
       </c>
       <c r="D60" s="25"/>
       <c r="E60" s="25"/>
@@ -3142,7 +3181,7 @@
         <v>87</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
@@ -3152,7 +3191,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B62" s="25" t="s">
         <v>83</v>
@@ -3184,7 +3223,7 @@
         <v>83</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25"/>
@@ -3196,7 +3235,7 @@
         <v>97</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C65" s="25"/>
       <c r="D65" s="25"/>
@@ -3209,7 +3248,7 @@
         <v>112</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>100</v>
@@ -3235,10 +3274,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>100</v>
@@ -3259,7 +3298,7 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B70" s="25"/>
       <c r="C70" s="25"/>
@@ -3270,7 +3309,7 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B71" s="25" t="s">
         <v>83</v>
@@ -3322,31 +3361,31 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B82" t="s">
         <v>85</v>
       </c>
       <c r="C82" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
+        <v>260</v>
+      </c>
+      <c r="B84" t="s">
         <v>261</v>
-      </c>
-      <c r="B84" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B85" t="s">
         <v>85</v>
@@ -3354,7 +3393,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B86" t="s">
         <v>85</v>
@@ -3362,32 +3401,32 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3460,7 +3499,7 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B101" s="25"/>
       <c r="C101" s="25"/>
@@ -3473,7 +3512,7 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B102" s="25"/>
       <c r="C102" s="25"/>
@@ -3486,10 +3525,10 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B103" s="25" t="s">
         <v>212</v>
-      </c>
-      <c r="B103" s="25" t="s">
-        <v>213</v>
       </c>
       <c r="C103" s="25"/>
       <c r="D103" s="25"/>
@@ -3501,13 +3540,13 @@
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="B104" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B104" s="25" t="s">
+      <c r="C104" s="25" t="s">
         <v>215</v>
-      </c>
-      <c r="C104" s="25" t="s">
-        <v>216</v>
       </c>
       <c r="D104" s="25"/>
       <c r="E104" s="25"/>
@@ -3531,18 +3570,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
     <col min="16" max="16" width="13.5" customWidth="1"/>
     <col min="17" max="17" width="17.1640625" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="20" max="20" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -3562,16 +3603,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="L1" t="s">
         <v>57</v>
@@ -3613,7 +3654,7 @@
         <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -3628,7 +3669,7 @@
         <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L4" t="s">
         <v>55</v>
@@ -3657,7 +3698,7 @@
         <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D5">
         <v>18</v>
@@ -3672,7 +3713,7 @@
         <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L5" t="s">
         <v>56</v>
@@ -3701,7 +3742,7 @@
         <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D6">
         <v>17.25</v>
@@ -3716,7 +3757,7 @@
         <v>86</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -3727,7 +3768,7 @@
         <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -3742,7 +3783,7 @@
         <v>86</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L7" t="s">
         <v>57</v>
@@ -3795,7 +3836,7 @@
         <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -3821,7 +3862,7 @@
         <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -3832,7 +3873,7 @@
         <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D10">
         <v>18.5</v>
@@ -3847,34 +3888,37 @@
         <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="D11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="16" thickBot="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="17" thickTop="1" thickBot="1">
+      <c r="B14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>361</v>
       </c>
       <c r="B15" t="s">
         <v>144</v>
       </c>
-      <c r="C15" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="D15" s="31">
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15">
         <v>11.5</v>
       </c>
-      <c r="E15" s="31">
-        <v>15.5</v>
+      <c r="E15" t="s">
+        <v>347</v>
       </c>
       <c r="F15" t="s">
         <v>83</v>
@@ -3883,10 +3927,10 @@
         <v>86</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="16" thickTop="1">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -3894,7 +3938,7 @@
         <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16">
         <v>12.5</v>
@@ -3909,7 +3953,7 @@
         <v>91</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -3920,7 +3964,7 @@
         <v>126</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D17">
         <v>8.5</v>
@@ -3935,7 +3979,7 @@
         <v>86</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I17" s="24"/>
       <c r="K17" s="24"/>
@@ -3990,7 +4034,7 @@
         <v>143</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D18">
         <v>8.5</v>
@@ -3999,13 +4043,13 @@
         <v>6</v>
       </c>
       <c r="F18" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="G18" s="23" t="s">
-        <v>171</v>
-      </c>
       <c r="H18" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L18" t="s">
         <v>56</v>
@@ -4048,16 +4092,19 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19" t="s">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
-      </c>
-      <c r="D19" t="s">
-        <v>331</v>
+        <v>182</v>
+      </c>
+      <c r="D19">
+        <v>11.5</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>83</v>
@@ -4066,20 +4113,20 @@
         <v>86</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" t="s">
         <v>162</v>
-      </c>
-      <c r="B23" t="s">
-        <v>163</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -4099,10 +4146,10 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
@@ -4122,10 +4169,10 @@
     </row>
     <row r="25" spans="1:24">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
@@ -4137,7 +4184,7 @@
         <v>12.5</v>
       </c>
       <c r="F25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G25" t="s">
         <v>83</v>
@@ -4152,7 +4199,7 @@
     </row>
     <row r="28" spans="1:24">
       <c r="A28" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
@@ -4162,13 +4209,13 @@
     </row>
     <row r="29" spans="1:24">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
         <v>129</v>
       </c>
       <c r="C29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -4177,13 +4224,13 @@
         <v>4.5</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H29" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I29" s="24"/>
       <c r="J29" s="24"/>
@@ -4191,13 +4238,13 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
         <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -4206,13 +4253,13 @@
         <v>4.5</v>
       </c>
       <c r="F30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M30">
         <f>36-N30</f>
@@ -4231,7 +4278,7 @@
         <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D31">
         <v>9</v>
@@ -4246,18 +4293,18 @@
         <v>86</v>
       </c>
       <c r="H31" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:24">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D32">
         <v>8</v>
@@ -4269,21 +4316,21 @@
         <v>83</v>
       </c>
       <c r="G32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D33">
         <v>8</v>
@@ -4298,18 +4345,18 @@
         <v>86</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D34">
         <v>1.5</v>
@@ -4318,18 +4365,18 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G34" t="s">
         <v>86</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="36" spans="1:18">
       <c r="L36" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>67</v>
@@ -4338,18 +4385,18 @@
         <v>3</v>
       </c>
       <c r="O36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" t="s">
         <v>158</v>
-      </c>
-      <c r="C37" t="s">
-        <v>159</v>
       </c>
       <c r="D37">
         <v>7.5</v>
@@ -4364,13 +4411,13 @@
         <v>86</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N37" s="6">
         <v>1</v>
@@ -4381,10 +4428,10 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" t="s">
         <v>158</v>
-      </c>
-      <c r="C38" t="s">
-        <v>159</v>
       </c>
       <c r="D38">
         <v>7.5</v>
@@ -4399,10 +4446,10 @@
         <v>86</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L38" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M38" s="28" t="s">
         <v>69</v>
@@ -4411,12 +4458,12 @@
         <v>1</v>
       </c>
       <c r="O38" s="29" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B39" s="25" t="s">
         <v>128</v>
@@ -4431,19 +4478,19 @@
         <v>1</v>
       </c>
       <c r="F39" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="G39" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>174</v>
-      </c>
       <c r="H39" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L39" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="M39" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="N39" s="27">
         <v>2</v>
@@ -4451,13 +4498,13 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D40">
         <v>1.25</v>
@@ -4469,24 +4516,24 @@
         <v>83</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I40" s="25"/>
       <c r="J40" s="25"/>
       <c r="K40" s="25"/>
       <c r="Q40" t="s">
+        <v>320</v>
+      </c>
+      <c r="R40" t="s">
         <v>321</v>
-      </c>
-      <c r="R40" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="41" spans="1:18">
       <c r="C41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D41">
         <v>1.25</v>
@@ -4495,10 +4542,10 @@
         <v>1.25</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L41" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M41" s="1" t="s">
         <v>73</v>
@@ -4507,10 +4554,10 @@
         <v>1</v>
       </c>
       <c r="O41" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q41" s="27" t="s">
         <v>310</v>
-      </c>
-      <c r="Q41" s="27" t="s">
-        <v>311</v>
       </c>
       <c r="R41" s="27" t="s">
         <v>85</v>
@@ -4518,22 +4565,22 @@
     </row>
     <row r="42" spans="1:18">
       <c r="L42" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" spans="1:18">
       <c r="A43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N43" s="27">
         <v>1</v>
       </c>
       <c r="O43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>83</v>
@@ -4544,15 +4591,15 @@
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L45" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M45" s="12" t="s">
         <v>68</v>
@@ -4563,16 +4610,16 @@
     </row>
     <row r="46" spans="1:18">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L46" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="N46" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="N46" s="1" t="s">
-        <v>301</v>
-      </c>
       <c r="P46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q46" t="s">
         <v>83</v>
@@ -4583,13 +4630,13 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q47" t="s">
         <v>83</v>
@@ -4598,21 +4645,21 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L49" t="s">
         <v>71</v>
       </c>
       <c r="M49" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="N49">
         <v>1</v>
       </c>
       <c r="P49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q49" t="s">
         <v>83</v>
@@ -4621,75 +4668,80 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:21">
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L50" t="s">
         <v>70</v>
       </c>
       <c r="M50" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
       <c r="A52" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:21">
-      <c r="A53" t="s">
+    <row r="55" spans="1:22">
+      <c r="A55" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="55" spans="1:21">
-      <c r="A55" t="s">
-        <v>202</v>
-      </c>
       <c r="H55" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="K55" s="18"/>
       <c r="L55" s="1" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="M55" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="N55" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="N55" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="O55" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="T55" s="33" t="s">
         <v>325</v>
       </c>
-      <c r="Q55" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="R55" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1" t="s">
-        <v>326</v>
-      </c>
       <c r="U55" s="1"/>
-    </row>
-    <row r="56" spans="1:21">
+      <c r="V55" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K56" s="18"/>
       <c r="L56" s="27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M56" s="27" t="s">
         <v>88</v>
@@ -4706,26 +4758,29 @@
       <c r="R56">
         <v>-28</v>
       </c>
-      <c r="T56">
+      <c r="S56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:21">
+      <c r="T56" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22">
       <c r="H57" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I57" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="K57" s="18"/>
       <c r="L57" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M57" s="27" t="s">
         <v>85</v>
       </c>
       <c r="N57" s="27" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O57">
         <v>10</v>
@@ -4736,23 +4791,29 @@
       <c r="R57">
         <v>-8</v>
       </c>
-      <c r="T57">
+      <c r="S57">
         <v>12</v>
       </c>
+      <c r="T57" s="32">
+        <v>16</v>
+      </c>
       <c r="U57" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21">
+        <v>335</v>
+      </c>
+      <c r="V57" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22">
       <c r="H58" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="I58" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="K58" s="18"/>
       <c r="L58" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M58" s="27" t="s">
         <v>85</v>
@@ -4766,37 +4827,44 @@
       <c r="Q58" s="23">
         <v>16</v>
       </c>
-      <c r="R58" s="32">
+      <c r="R58" s="31">
         <v>0</v>
       </c>
-      <c r="T58">
+      <c r="S58">
         <v>16</v>
       </c>
+      <c r="T58" s="32" t="s">
+        <v>358</v>
+      </c>
       <c r="U58" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21">
+        <v>334</v>
+      </c>
+      <c r="V58" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22">
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
       <c r="M59" s="18"/>
       <c r="N59" s="18"/>
       <c r="O59" s="18"/>
       <c r="P59" s="18"/>
-    </row>
-    <row r="60" spans="1:21">
+      <c r="T59" s="32"/>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" t="s">
         <v>116</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K60" s="18"/>
       <c r="L60" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M60" s="27" t="s">
         <v>83</v>
@@ -4814,20 +4882,23 @@
       <c r="R60">
         <v>-9</v>
       </c>
-    </row>
-    <row r="61" spans="1:21">
+      <c r="T60" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22">
       <c r="A61" t="s">
         <v>117</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K61" s="18"/>
       <c r="L61" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M61" s="27" t="s">
         <v>83</v>
@@ -4845,8 +4916,11 @@
       <c r="R61">
         <v>-9</v>
       </c>
-    </row>
-    <row r="62" spans="1:21">
+      <c r="T61" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22">
       <c r="A62" t="s">
         <v>118</v>
       </c>
@@ -4856,8 +4930,9 @@
       <c r="N62" s="18"/>
       <c r="O62" s="18"/>
       <c r="P62" s="18"/>
-    </row>
-    <row r="63" spans="1:21">
+      <c r="T62" s="32"/>
+    </row>
+    <row r="63" spans="1:22">
       <c r="A63" t="s">
         <v>119</v>
       </c>
@@ -4865,11 +4940,11 @@
         <v>71</v>
       </c>
       <c r="I63" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="K63" s="18"/>
       <c r="L63" s="27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M63" s="27" t="s">
         <v>83</v>
@@ -4887,45 +4962,57 @@
       <c r="R63">
         <v>-7</v>
       </c>
-    </row>
-    <row r="64" spans="1:21">
+      <c r="S63">
+        <v>9</v>
+      </c>
+      <c r="T63" s="32">
+        <v>9</v>
+      </c>
+      <c r="U63" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
       <c r="A64" t="s">
         <v>120</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I64" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="K64" s="18"/>
       <c r="L64" s="27" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="M64" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N64" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O64" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P64" s="18"/>
-      <c r="Q64" s="32" t="s">
-        <v>289</v>
+      <c r="Q64" s="31" t="s">
+        <v>288</v>
       </c>
       <c r="R64" s="23">
         <v>0</v>
       </c>
-      <c r="T64">
+      <c r="S64">
         <v>8</v>
       </c>
+      <c r="T64" s="32">
+        <v>20</v>
+      </c>
       <c r="U64" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65" t="s">
         <v>121</v>
       </c>
@@ -4936,25 +5023,58 @@
       <c r="O65" s="18"/>
       <c r="P65" s="18"/>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:18">
       <c r="I66" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L66" s="27" t="s">
         <v>70</v>
       </c>
       <c r="M66" s="27" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16">
+        <v>333</v>
+      </c>
+      <c r="O66" t="s">
+        <v>352</v>
+      </c>
+      <c r="P66" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q66">
+        <f>12*4</f>
+        <v>48</v>
+      </c>
+      <c r="R66" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67" t="s">
+        <v>189</v>
+      </c>
+      <c r="O67" t="s">
+        <v>353</v>
+      </c>
+      <c r="P67" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q67">
+        <f>15*4</f>
+        <v>60</v>
+      </c>
+      <c r="R67" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="A68" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="68" spans="1:16">
-      <c r="A68" t="s">
-        <v>191</v>
+      <c r="Q68">
+        <f>96-60</f>
+        <v>36</v>
+      </c>
+      <c r="R68" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted captured acrylic pieces for side_frame and both attachments, slotted and door
</commit_message>
<xml_diff>
--- a/instructions/behav_rig_specs_final.xlsx
+++ b/instructions/behav_rig_specs_final.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27740" yWindow="5500" windowWidth="23500" windowHeight="12860" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="800" yWindow="380" windowWidth="20520" windowHeight="12920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="acrylic pieces" sheetId="1" r:id="rId1"/>
@@ -3571,7 +3571,7 @@
   <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
adding detailed readme. updated construction notes. added helpful images
</commit_message>
<xml_diff>
--- a/instructions/behav_rig_specs_final.xlsx
+++ b/instructions/behav_rig_specs_final.xlsx
@@ -1,18 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julianarhee/Repositories/behavior_rig/instructions/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB37DA3-1714-0D44-91F8-8DEA77304148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="380" windowWidth="20520" windowHeight="12920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="800" yWindow="760" windowWidth="26680" windowHeight="16480" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="acrylic pieces" sheetId="1" r:id="rId1"/>
+    <sheet name="acrylic piece sizes to order" sheetId="1" r:id="rId1"/>
     <sheet name="accessory pieces" sheetId="2" r:id="rId2"/>
     <sheet name="finalized pieces " sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="364">
   <si>
     <t>Base</t>
   </si>
@@ -1131,11 +1148,17 @@
   <si>
     <t>side door (attachment) (M6 thumb or 4 M3 tapped)</t>
   </si>
+  <si>
+    <t>Bulk Piece Assignments:</t>
+  </si>
+  <si>
+    <t>Estimated Bulk Acrylic Pieces to Order:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1477,14 +1500,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1496,20 +1518,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="23"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="114"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="114" applyFont="1"/>
   </cellXfs>
@@ -1636,6 +1653,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1960,24 +1985,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E9"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.5" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -1993,23 +2018,26 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>54</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2031,26 +2059,26 @@
       <c r="H2" t="s">
         <v>71</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>55</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <f>E2</f>
         <v>18.5</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <f>D4</f>
         <v>17.25</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>8</v>
       </c>
-      <c r="O2">
-        <f>J2+K2</f>
+      <c r="P2">
+        <f>K2+L2</f>
         <v>35.75</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2072,26 +2100,26 @@
       <c r="H3" t="s">
         <v>71</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>56</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f>D2</f>
         <v>18</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f>E4</f>
         <v>8.8249999999999993</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3">
-        <f>K3+L3+M3</f>
+      <c r="P3">
+        <f>L3+M3+N3</f>
         <v>9.8249999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2114,7 +2142,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2136,35 +2164,35 @@
       <c r="H5" t="s">
         <v>74</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>57</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>61</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>62</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>63</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>8</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>65</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>66</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2186,50 +2214,50 @@
       <c r="H6" t="s">
         <v>74</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>55</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f>E3</f>
         <v>18.5</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f>E10*2</f>
         <v>9</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>8.5</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>8.25</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>5</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>3</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>9</v>
       </c>
-      <c r="R6">
-        <f>SUM(J6:L6)</f>
+      <c r="S6">
+        <f>SUM(K6:M6)</f>
         <v>36</v>
       </c>
-      <c r="S6">
-        <f>SUM(J6,K6,M6)</f>
+      <c r="T6">
+        <f>SUM(K6,L6,N6)</f>
         <v>35.75</v>
       </c>
-      <c r="T6">
-        <f>SUM(J6,K6,N6,O6)</f>
+      <c r="U6">
+        <f>SUM(K6,L6,O6,P6)</f>
         <v>35.5</v>
       </c>
-      <c r="U6">
-        <f>SUM(J6,P6,N6,O6)</f>
+      <c r="V6">
+        <f>SUM(K6,Q6,O6,P6)</f>
         <v>35.5</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2251,46 +2279,46 @@
       <c r="H7" t="s">
         <v>74</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>56</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f>D3</f>
         <v>18</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f>D10*3</f>
         <v>15</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>6</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>4</v>
-      </c>
-      <c r="N7">
-        <v>8</v>
       </c>
       <c r="O7">
         <v>8</v>
       </c>
       <c r="P7">
+        <v>8</v>
+      </c>
+      <c r="Q7">
         <v>1.5</v>
       </c>
-      <c r="R7">
-        <f>SUM(L7,M7,N7)</f>
+      <c r="S7">
+        <f>SUM(M7,N7,O7)</f>
         <v>18</v>
       </c>
-      <c r="S7">
-        <f>SUM(K7,P7)</f>
+      <c r="T7">
+        <f>SUM(L7,Q7)</f>
         <v>16.5</v>
       </c>
-      <c r="T7">
-        <f>SUM(L7,M7,O7)</f>
+      <c r="U7">
+        <f>SUM(M7,N7,P7)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2316,7 +2344,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2341,16 +2369,16 @@
       <c r="H9" t="s">
         <v>71</v>
       </c>
-      <c r="J9">
-        <f>36-K9</f>
+      <c r="K9">
+        <f>36-L9</f>
         <v>8.5</v>
       </c>
-      <c r="K9">
-        <f>J6+K6</f>
+      <c r="L9">
+        <f>K6+L6</f>
         <v>27.5</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2376,7 +2404,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2402,7 +2430,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -2421,19 +2449,22 @@
       <c r="H12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="I13" s="2" t="s">
+      <c r="J12" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="4">
+      <c r="L13" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2452,17 +2483,17 @@
       <c r="F14" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="K14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K14" s="7">
+      <c r="L14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2478,17 +2509,17 @@
       <c r="E15">
         <v>8</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="K15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K15" s="10">
+      <c r="L15" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2505,7 +2536,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2521,23 +2552,23 @@
       <c r="E17">
         <v>3.5</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <f>36-11</f>
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="I18" s="11" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J18" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="K18" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="K18" s="13">
+      <c r="L18" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2557,7 +2588,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2577,7 +2608,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -2596,20 +2627,20 @@
       <c r="F23" t="s">
         <v>76</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f>18.5+17.5</f>
         <v>36</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f>36-19</f>
         <v>17</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <f>9/1.5</f>
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2628,16 +2659,16 @@
       <c r="F24" t="s">
         <v>75</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f>7.5*2</f>
         <v>15</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f>16.5+9</f>
         <v>25.5</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2657,7 +2688,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -2676,8 +2707,11 @@
       <c r="F26" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="J26" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2696,54 +2730,54 @@
       <c r="F27" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="J27" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="K27" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K27" s="16">
+      <c r="L27" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
-      <c r="I28" s="17" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="K28" t="s">
         <v>81</v>
       </c>
-      <c r="K28" s="19">
+      <c r="L28" s="17">
         <v>3</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <f>8.5*2</f>
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
-      <c r="I29" s="17" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J29" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J29" s="18" t="s">
+      <c r="K29" t="s">
         <v>78</v>
       </c>
-      <c r="K29" s="19">
+      <c r="L29" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="I30" s="20" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J30" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="J30" s="21" t="s">
+      <c r="K30" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="K30" s="22">
+      <c r="L30" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E31">
         <f>15+18.5</f>
         <v>33.5</v>
@@ -2757,7 +2791,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E32">
         <f>18.5+13</f>
         <v>31.5</v>
@@ -2779,36 +2813,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55.1640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -2819,13 +2853,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>239</v>
       </c>
       <c r="B8" t="s">
@@ -2835,7 +2869,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>256</v>
       </c>
@@ -2846,7 +2880,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>221</v>
       </c>
@@ -2857,13 +2891,13 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>216</v>
       </c>
       <c r="B13" t="s">
@@ -2873,8 +2907,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>222</v>
       </c>
       <c r="B14" t="s">
@@ -2884,8 +2918,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>223</v>
       </c>
       <c r="B15" t="s">
@@ -2895,8 +2929,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>224</v>
       </c>
       <c r="B16" t="s">
@@ -2906,7 +2940,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>225</v>
       </c>
@@ -2917,23 +2951,23 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>245</v>
       </c>
       <c r="B18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="25"/>
-    </row>
-    <row r="20" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>229</v>
       </c>
@@ -2944,7 +2978,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2955,12 +2989,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="D23" s="25" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="22" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>228</v>
       </c>
@@ -2971,7 +3005,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>207</v>
       </c>
@@ -2979,7 +3013,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>230</v>
       </c>
@@ -2990,7 +3024,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>232</v>
       </c>
@@ -2998,7 +3032,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>233</v>
       </c>
@@ -3006,7 +3040,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>234</v>
       </c>
@@ -3017,8 +3051,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="23" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>235</v>
       </c>
       <c r="B32" t="s">
@@ -3028,13 +3062,13 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="23" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>242</v>
       </c>
       <c r="B35" t="s">
@@ -3044,20 +3078,20 @@
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>280</v>
       </c>
@@ -3068,7 +3102,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -3076,7 +3110,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -3087,12 +3121,12 @@
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>252</v>
       </c>
@@ -3103,22 +3137,22 @@
         <v>253</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -3126,7 +3160,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>275</v>
       </c>
@@ -3134,232 +3168,232 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="26" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="25" t="s">
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="B59" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C59" s="25" t="s">
+      <c r="C59" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="25" t="s">
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="B60" s="25" t="s">
+      <c r="B60" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="25" t="s">
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="25" t="s">
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="25" t="s">
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="25" t="s">
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C64" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="25" t="s">
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="25" t="s">
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="B66" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="C66" s="25" t="s">
+      <c r="C66" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="25" t="s">
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B67" s="25" t="s">
+      <c r="B67" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="25" t="s">
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B68" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="25"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="26" t="s">
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="22"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="25" t="s">
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="B71" s="25" t="s">
+      <c r="B71" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="25"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="25"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="25"/>
-      <c r="B77" s="25"/>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="22"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="22"/>
+      <c r="B77" s="22"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>257</v>
       </c>
@@ -3370,12 +3404,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>260</v>
       </c>
@@ -3383,7 +3417,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>267</v>
       </c>
@@ -3391,7 +3425,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>268</v>
       </c>
@@ -3399,161 +3433,161 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="24" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="21" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="25" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B97" s="25" t="s">
+      <c r="B97" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C97" s="25" t="s">
+      <c r="C97" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="25"/>
-      <c r="H97" s="25"/>
-      <c r="I97" s="25"/>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="25" t="s">
+      <c r="D97" s="22"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="22"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B98" s="25" t="s">
+      <c r="B98" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C98" s="25" t="s">
+      <c r="C98" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="25"/>
-      <c r="H98" s="25"/>
-      <c r="I98" s="25"/>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99" s="25" t="s">
+      <c r="D98" s="22"/>
+      <c r="E98" s="22"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="22"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="B99" s="25" t="s">
+      <c r="B99" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="C99" s="25" t="s">
+      <c r="C99" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="25"/>
-      <c r="G99" s="25"/>
-      <c r="H99" s="25"/>
-      <c r="I99" s="25"/>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="25" t="s">
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="25" t="s">
+      <c r="B100" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C100" s="25" t="s">
+      <c r="C100" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
-      <c r="H100" s="25"/>
-      <c r="I100" s="25"/>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" s="25" t="s">
+      <c r="D100" s="22"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
+      <c r="H100" s="22"/>
+      <c r="I100" s="22"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="B101" s="25"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="25"/>
-      <c r="H101" s="25"/>
-      <c r="I101" s="25"/>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" s="25" t="s">
+      <c r="B101" s="22"/>
+      <c r="C101" s="22"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
+      <c r="H101" s="22"/>
+      <c r="I101" s="22"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25"/>
-      <c r="H102" s="25"/>
-      <c r="I102" s="25"/>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="25" t="s">
+      <c r="B102" s="22"/>
+      <c r="C102" s="22"/>
+      <c r="D102" s="22"/>
+      <c r="E102" s="22"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="22"/>
+      <c r="H102" s="22"/>
+      <c r="I102" s="22"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="B103" s="25" t="s">
+      <c r="B103" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="25"/>
-      <c r="H103" s="25"/>
-      <c r="I103" s="25"/>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="25" t="s">
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="22"/>
+      <c r="G103" s="22"/>
+      <c r="H103" s="22"/>
+      <c r="I103" s="22"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="B104" s="25" t="s">
+      <c r="B104" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="C104" s="25" t="s">
+      <c r="C104" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="25"/>
-      <c r="H104" s="25"/>
-      <c r="I104" s="25"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22"/>
+      <c r="G104" s="22"/>
+      <c r="H104" s="22"/>
+      <c r="I104" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3567,14 +3601,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="43.5" customWidth="1"/>
@@ -3586,7 +3620,7 @@
     <col min="20" max="20" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -3630,14 +3664,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -3646,7 +3680,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3690,7 +3724,7 @@
         <v>35.75</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3734,7 +3768,7 @@
         <v>9.8249999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3756,11 +3790,11 @@
       <c r="G6" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3813,7 +3847,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -3839,7 +3873,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -3865,7 +3899,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -3891,12 +3925,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>142</v>
       </c>
@@ -3904,7 +3938,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>361</v>
       </c>
@@ -3930,7 +3964,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -3956,14 +3990,14 @@
         <v>304</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="22" t="s">
         <v>183</v>
       </c>
       <c r="D17">
@@ -3972,17 +4006,17 @@
       <c r="E17">
         <v>6</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" t="s">
         <v>86</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="K17" s="24"/>
+      <c r="I17" s="21"/>
+      <c r="K17" s="21"/>
       <c r="L17" t="s">
         <v>55</v>
       </c>
@@ -4026,14 +4060,14 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>127</v>
       </c>
       <c r="B18" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="22" t="s">
         <v>183</v>
       </c>
       <c r="D18">
@@ -4042,13 +4076,13 @@
       <c r="E18">
         <v>6</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" t="s">
         <v>169</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" t="s">
         <v>170</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" t="s">
         <v>288</v>
       </c>
       <c r="L18" t="s">
@@ -4090,7 +4124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>328</v>
       </c>
@@ -4106,23 +4140,23 @@
       <c r="E19">
         <v>15</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" t="s">
         <v>86</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>161</v>
       </c>
       <c r="B23" t="s">
@@ -4144,20 +4178,20 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" t="s">
         <v>285</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24">
         <v>18.5</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24">
         <v>12.5</v>
       </c>
       <c r="F24" t="s">
@@ -4167,20 +4201,20 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" t="s">
         <v>163</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25">
         <v>18.5</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25">
         <v>12.5</v>
       </c>
       <c r="F25" t="s">
@@ -4190,24 +4224,24 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -4226,17 +4260,17 @@
       <c r="F29" t="s">
         <v>171</v>
       </c>
-      <c r="G29" s="23" t="s">
+      <c r="G29" t="s">
         <v>180</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="H29" t="s">
         <v>180</v>
       </c>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-    </row>
-    <row r="30" spans="1:24">
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -4270,7 +4304,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>131</v>
       </c>
@@ -4292,11 +4326,11 @@
       <c r="G31" t="s">
         <v>86</v>
       </c>
-      <c r="H31" s="23" t="s">
+      <c r="H31" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>186</v>
       </c>
@@ -4322,7 +4356,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -4348,7 +4382,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -4374,21 +4408,21 @@
         <v>313</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
-      <c r="L36" s="6" t="s">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L36" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="M36" s="6" t="s">
+      <c r="M36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N36" s="1">
         <v>3</v>
       </c>
       <c r="O36" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>187</v>
       </c>
@@ -4410,20 +4444,20 @@
       <c r="G37" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="26" t="s">
+      <c r="H37" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="L37" s="6" t="s">
+      <c r="L37" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="M37" s="6" t="s">
+      <c r="M37" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="N37" s="6">
+      <c r="N37" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -4445,45 +4479,45 @@
       <c r="G38" t="s">
         <v>86</v>
       </c>
-      <c r="H38" s="26" t="s">
+      <c r="H38" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="L38" s="28" t="s">
+      <c r="L38" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="M38" s="28" t="s">
+      <c r="M38" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="N38" s="28">
+      <c r="N38" s="24">
         <v>1</v>
       </c>
-      <c r="O38" s="29" t="s">
+      <c r="O38" s="25" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
-      <c r="A39" s="25" t="s">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="D39" s="25">
+      <c r="D39" s="22">
         <v>1.6</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="22">
         <v>1</v>
       </c>
-      <c r="F39" s="25" t="s">
+      <c r="F39" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G39" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="H39" s="25" t="s">
+      <c r="H39" s="22" t="s">
         <v>185</v>
       </c>
       <c r="L39" s="1" t="s">
@@ -4492,11 +4526,11 @@
       <c r="M39" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="N39" s="27">
+      <c r="N39" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>286</v>
       </c>
@@ -4515,15 +4549,15 @@
       <c r="F40" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="25" t="s">
+      <c r="G40" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="H40" s="26" t="s">
+      <c r="H40" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
       <c r="Q40" t="s">
         <v>320</v>
       </c>
@@ -4531,7 +4565,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>182</v>
       </c>
@@ -4544,31 +4578,31 @@
       <c r="H41" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="L41" s="27" t="s">
+      <c r="L41" s="1" t="s">
         <v>308</v>
       </c>
       <c r="M41" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N41" s="27">
+      <c r="N41" s="1">
         <v>1</v>
       </c>
       <c r="O41" t="s">
         <v>309</v>
       </c>
-      <c r="Q41" s="27" t="s">
+      <c r="Q41" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="R41" s="27" t="s">
+      <c r="R41" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L42" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="L43" s="1" t="s">
         <v>319</v>
@@ -4576,7 +4610,7 @@
       <c r="M43" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="N43" s="27">
+      <c r="N43" s="1">
         <v>1</v>
       </c>
       <c r="O43" t="s">
@@ -4589,30 +4623,30 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>193</v>
       </c>
-      <c r="L45" s="11" t="s">
+      <c r="L45" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="M45" s="12" t="s">
+      <c r="M45" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="N45" s="13">
+      <c r="N45" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>195</v>
       </c>
-      <c r="L46" s="27" t="s">
+      <c r="L46" s="1" t="s">
         <v>299</v>
       </c>
       <c r="N46" s="1" t="s">
@@ -4628,7 +4662,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>194</v>
       </c>
@@ -4645,7 +4679,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:22">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>196</v>
       </c>
@@ -4668,7 +4702,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>197</v>
       </c>
@@ -4679,17 +4713,17 @@
         <v>333</v>
       </c>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="1:22">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:22">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>201</v>
       </c>
@@ -4699,7 +4733,6 @@
       <c r="I55" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="K55" s="18"/>
       <c r="L55" s="1" t="s">
         <v>341</v>
       </c>
@@ -4721,7 +4754,7 @@
       <c r="S55" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="T55" s="33" t="s">
+      <c r="T55" s="27" t="s">
         <v>325</v>
       </c>
       <c r="U55" s="1"/>
@@ -4729,7 +4762,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="56" spans="1:22">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>202</v>
       </c>
@@ -4739,14 +4772,13 @@
       <c r="I56" t="s">
         <v>195</v>
       </c>
-      <c r="K56" s="18"/>
-      <c r="L56" s="27" t="s">
+      <c r="L56" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="M56" s="27" t="s">
+      <c r="M56" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N56" s="27" t="s">
+      <c r="N56" s="1" t="s">
         <v>93</v>
       </c>
       <c r="O56">
@@ -4761,25 +4793,24 @@
       <c r="S56">
         <v>0</v>
       </c>
-      <c r="T56" s="32">
+      <c r="T56" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:22">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H57" s="1" t="s">
         <v>291</v>
       </c>
       <c r="I57" t="s">
         <v>336</v>
       </c>
-      <c r="K57" s="18"/>
       <c r="L57" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="M57" s="27" t="s">
+      <c r="M57" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N57" s="27" t="s">
+      <c r="N57" s="1" t="s">
         <v>322</v>
       </c>
       <c r="O57">
@@ -4794,7 +4825,7 @@
       <c r="S57">
         <v>12</v>
       </c>
-      <c r="T57" s="32">
+      <c r="T57" s="26">
         <v>16</v>
       </c>
       <c r="U57" t="s">
@@ -4804,36 +4835,35 @@
         <v>342</v>
       </c>
     </row>
-    <row r="58" spans="1:22">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H58" s="1" t="s">
         <v>338</v>
       </c>
       <c r="I58" t="s">
         <v>337</v>
       </c>
-      <c r="K58" s="18"/>
       <c r="L58" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="M58" s="27" t="s">
+      <c r="M58" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N58" s="27" t="s">
+      <c r="N58" s="1" t="s">
         <v>91</v>
       </c>
       <c r="O58">
         <v>8</v>
       </c>
-      <c r="Q58" s="23">
+      <c r="Q58">
         <v>16</v>
       </c>
-      <c r="R58" s="31">
+      <c r="R58">
         <v>0</v>
       </c>
       <c r="S58">
         <v>16</v>
       </c>
-      <c r="T58" s="32" t="s">
+      <c r="T58" s="26" t="s">
         <v>358</v>
       </c>
       <c r="U58" t="s">
@@ -4843,16 +4873,10 @@
         <v>343</v>
       </c>
     </row>
-    <row r="59" spans="1:22">
-      <c r="K59" s="18"/>
-      <c r="L59" s="18"/>
-      <c r="M59" s="18"/>
-      <c r="N59" s="18"/>
-      <c r="O59" s="18"/>
-      <c r="P59" s="18"/>
-      <c r="T59" s="32"/>
-    </row>
-    <row r="60" spans="1:22">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T59" s="26"/>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -4862,31 +4886,29 @@
       <c r="I60" t="s">
         <v>196</v>
       </c>
-      <c r="K60" s="18"/>
-      <c r="L60" s="6" t="s">
+      <c r="L60" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="M60" s="27" t="s">
+      <c r="M60" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N60" s="27" t="s">
+      <c r="N60" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O60" s="30">
+      <c r="O60">
         <v>4</v>
       </c>
-      <c r="P60" s="18"/>
       <c r="Q60">
         <v>9</v>
       </c>
       <c r="R60">
         <v>-9</v>
       </c>
-      <c r="T60" s="32">
+      <c r="T60" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:22">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -4896,43 +4918,35 @@
       <c r="I61" t="s">
         <v>197</v>
       </c>
-      <c r="K61" s="18"/>
-      <c r="L61" s="27" t="s">
+      <c r="L61" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="M61" s="27" t="s">
+      <c r="M61" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N61" s="27" t="s">
+      <c r="N61" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O61" s="30">
+      <c r="O61">
         <v>4</v>
       </c>
-      <c r="P61" s="18"/>
       <c r="Q61">
         <v>9</v>
       </c>
       <c r="R61">
         <v>-9</v>
       </c>
-      <c r="T61" s="32">
+      <c r="T61" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:22">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>118</v>
       </c>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18"/>
-      <c r="N62" s="18"/>
-      <c r="O62" s="18"/>
-      <c r="P62" s="18"/>
-      <c r="T62" s="32"/>
-    </row>
-    <row r="63" spans="1:22">
+      <c r="T62" s="26"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>119</v>
       </c>
@@ -4942,20 +4956,18 @@
       <c r="I63" t="s">
         <v>349</v>
       </c>
-      <c r="K63" s="18"/>
-      <c r="L63" s="27" t="s">
+      <c r="L63" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="M63" s="27" t="s">
+      <c r="M63" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N63" s="27" t="s">
+      <c r="N63" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O63" s="30">
+      <c r="O63">
         <v>4</v>
       </c>
-      <c r="P63" s="18"/>
       <c r="Q63">
         <v>8</v>
       </c>
@@ -4965,14 +4977,14 @@
       <c r="S63">
         <v>9</v>
       </c>
-      <c r="T63" s="32">
+      <c r="T63" s="26">
         <v>9</v>
       </c>
       <c r="U63" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="64" spans="1:22">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -4982,55 +4994,47 @@
       <c r="I64" t="s">
         <v>348</v>
       </c>
-      <c r="K64" s="18"/>
-      <c r="L64" s="27" t="s">
+      <c r="L64" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="M64" s="27" t="s">
+      <c r="M64" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="N64" s="27" t="s">
+      <c r="N64" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="O64" s="27" t="s">
+      <c r="O64" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="P64" s="18"/>
-      <c r="Q64" s="31" t="s">
+      <c r="Q64" t="s">
         <v>288</v>
       </c>
-      <c r="R64" s="23">
+      <c r="R64">
         <v>0</v>
       </c>
       <c r="S64">
         <v>8</v>
       </c>
-      <c r="T64" s="32">
+      <c r="T64" s="26">
         <v>20</v>
       </c>
       <c r="U64" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>121</v>
       </c>
-      <c r="K65" s="18"/>
-      <c r="L65" s="18"/>
-      <c r="M65" s="18"/>
-      <c r="N65" s="18"/>
-      <c r="O65" s="18"/>
-      <c r="P65" s="18"/>
-    </row>
-    <row r="66" spans="1:18">
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I66" t="s">
         <v>198</v>
       </c>
-      <c r="L66" s="27" t="s">
+      <c r="L66" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M66" s="27" t="s">
+      <c r="M66" s="1" t="s">
         <v>333</v>
       </c>
       <c r="O66" t="s">
@@ -5047,7 +5051,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>189</v>
       </c>
@@ -5065,7 +5069,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>190</v>
       </c>

</xml_diff>